<commit_message>
Update plan term 2
</commit_message>
<xml_diff>
--- a/_document/Checklist - term2.xlsx
+++ b/_document/Checklist - term2.xlsx
@@ -75,9 +75,6 @@
     <t>Newest friends</t>
   </si>
   <si>
-    <t>Notification when cmt in my entry</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -109,13 +106,16 @@
   </si>
   <si>
     <t>Tags</t>
+  </si>
+  <si>
+    <t>Redirect to nowhere after comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +137,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -190,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -226,26 +219,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -264,20 +242,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -584,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="XBK9" sqref="XBK9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -599,17 +571,17 @@
   <sheetData>
     <row r="7" spans="1:31">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="8">
         <v>28</v>
@@ -702,7 +674,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="18"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -712,7 +684,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
-      <c r="V8" s="18"/>
+      <c r="V8" s="16"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -723,14 +695,14 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="2"/>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>27</v>
+      <c r="C9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -739,7 +711,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="18"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -749,7 +721,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="18"/>
+      <c r="V9" s="16"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -767,7 +739,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -776,7 +748,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="18"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -786,7 +758,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="18"/>
+      <c r="V10" s="16"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -797,14 +769,14 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="2"/>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>1.3</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>27</v>
+      <c r="D11" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -813,7 +785,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="18"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -823,7 +795,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="18"/>
+      <c r="V11" s="16"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -834,14 +806,14 @@
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="2"/>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>1.4</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
+      <c r="D12" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -850,7 +822,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="18"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -860,7 +832,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="18"/>
+      <c r="V12" s="16"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -878,7 +850,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -887,7 +859,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="18"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -897,7 +869,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="18"/>
+      <c r="V13" s="16"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -908,14 +880,14 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="2"/>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>1.6</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>27</v>
+      <c r="D14" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -924,7 +896,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -934,7 +906,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="18"/>
+      <c r="V14" s="16"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -945,14 +917,14 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="2"/>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>1.7</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>26</v>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -961,7 +933,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="18"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -971,7 +943,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="18"/>
+      <c r="V15" s="16"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -981,15 +953,15 @@
       <c r="AC15" s="2"/>
     </row>
     <row r="16" spans="1:31">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>28</v>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
@@ -1008,7 +980,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
-      <c r="V16" s="18"/>
+      <c r="V16" s="16"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
@@ -1018,15 +990,15 @@
       <c r="AC16" s="2"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>26</v>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
@@ -1045,7 +1017,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="18"/>
+      <c r="V17" s="16"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
@@ -1055,24 +1027,24 @@
       <c r="AC17" s="2"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="2">
+      <c r="A18" s="14">
         <v>4</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>27</v>
+      <c r="D18" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1082,7 +1054,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="V18" s="18"/>
+      <c r="V18" s="16"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -1092,15 +1064,15 @@
       <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="2">
+      <c r="A19" s="14">
         <v>5</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>27</v>
+      <c r="D19" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1109,17 +1081,17 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="18"/>
+      <c r="V19" s="16"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -1129,32 +1101,33 @@
       <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="20">
+      <c r="A20" s="14">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="20" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="S20" s="2"/>
+      <c r="V20" s="16"/>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="A21" s="1">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="S20" s="2"/>
-      <c r="V20" s="18"/>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="2">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1163,7 +1136,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="18"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1173,7 +1146,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="18"/>
+      <c r="V21" s="16"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
@@ -1198,17 +1171,17 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="18"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="18"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="16"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
@@ -1233,7 +1206,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="18"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1243,7 +1216,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="18"/>
+      <c r="V23" s="16"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
@@ -1268,7 +1241,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="18"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1278,7 +1251,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="18"/>
+      <c r="V24" s="16"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
@@ -1288,15 +1261,15 @@
       <c r="AC24" s="2"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>8</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>26</v>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1305,7 +1278,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="18"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -1315,7 +1288,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="19"/>
+      <c r="V25" s="17"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
@@ -1340,7 +1313,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="18"/>
+      <c r="L26" s="16"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1350,7 +1323,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="18"/>
+      <c r="V26" s="16"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
@@ -1375,7 +1348,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="18"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1385,7 +1358,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="18"/>
+      <c r="V27" s="16"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
@@ -1410,7 +1383,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="18"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1420,7 +1393,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="18"/>
+      <c r="V29" s="16"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
@@ -1445,7 +1418,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="18"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1455,7 +1428,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="18"/>
+      <c r="V30" s="16"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
@@ -1480,7 +1453,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="18"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1490,7 +1463,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-      <c r="V31" s="18"/>
+      <c r="V31" s="16"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
@@ -1508,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1517,7 +1490,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="18"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1527,7 +1500,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="V32" s="18"/>
+      <c r="V32" s="16"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>

</xml_diff>

<commit_message>
Checklist - term2.xlsx moi
</commit_message>
<xml_diff>
--- a/_document/Checklist - term2.xlsx
+++ b/_document/Checklist - term2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="120" windowWidth="15252" windowHeight="6048" activeTab="1"/>
+    <workbookView xWindow="90" yWindow="120" windowWidth="15255" windowHeight="6045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -119,7 +119,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,14 +127,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -229,9 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -248,6 +245,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,7 +546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -556,34 +556,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="6" max="29" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="4.625" customWidth="1"/>
+    <col min="3" max="3" width="28.375" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="4.375" customWidth="1"/>
+    <col min="6" max="29" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:31">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:31" ht="15">
+      <c r="A7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>28</v>
       </c>
       <c r="G7" s="2">
@@ -592,7 +593,7 @@
       <c r="H7" s="1">
         <v>30</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>31</v>
       </c>
       <c r="J7" s="2">
@@ -655,7 +656,7 @@
       <c r="AC7" s="1">
         <v>20</v>
       </c>
-      <c r="AD7" s="9"/>
+      <c r="AD7" s="8"/>
       <c r="AE7" s="2"/>
     </row>
     <row r="8" spans="1:31">
@@ -663,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2"/>
@@ -674,17 +675,17 @@
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="16"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="15"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -695,33 +696,33 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="2"/>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="16"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="15"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="16"/>
+      <c r="V9" s="15"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -741,24 +742,24 @@
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="16"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="16"/>
+      <c r="V10" s="15"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -769,33 +770,33 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="2"/>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>1.3</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="16"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="O11" s="15"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="16"/>
+      <c r="V11" s="15"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -806,13 +807,13 @@
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="2"/>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>1.4</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="2"/>
@@ -822,17 +823,17 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="16"/>
+      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="O12" s="15"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="16"/>
+      <c r="V12" s="15"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -852,24 +853,24 @@
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="16"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="O13" s="15"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="16"/>
+      <c r="V13" s="15"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -880,13 +881,13 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="2"/>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>1.6</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="2"/>
@@ -896,17 +897,17 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="16"/>
+      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="O14" s="15"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="16"/>
+      <c r="V14" s="15"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -917,7 +918,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="2"/>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>1.7</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -933,17 +934,17 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="16"/>
+      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="O15" s="15"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="16"/>
+      <c r="V15" s="15"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -973,14 +974,14 @@
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="15"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
-      <c r="V16" s="16"/>
+      <c r="V16" s="15"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
@@ -1010,14 +1011,14 @@
       <c r="L17" s="3"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="O17" s="15"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="16"/>
+      <c r="V17" s="15"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
@@ -1027,34 +1028,34 @@
       <c r="AC17" s="2"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>4</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="O18" s="15"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="V18" s="16"/>
+      <c r="V18" s="15"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -1064,14 +1065,14 @@
       <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <v>5</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="2"/>
@@ -1081,17 +1082,17 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="16"/>
+      <c r="V19" s="15"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -1101,22 +1102,22 @@
       <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="14">
+      <c r="A20" s="13">
         <v>6</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="S20" s="2"/>
-      <c r="V20" s="16"/>
+      <c r="V20" s="15"/>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1">
@@ -1129,14 +1130,14 @@
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="16"/>
+      <c r="L21" s="2"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1146,7 +1147,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="16"/>
+      <c r="V21" s="15"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
@@ -1160,7 +1161,7 @@
       <c r="B22" s="2">
         <v>7.1</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2"/>
@@ -1171,17 +1172,17 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="16"/>
+      <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="16"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="15"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
@@ -1195,7 +1196,7 @@
       <c r="B23" s="2">
         <v>7.2</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="2"/>
@@ -1206,17 +1207,17 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="16"/>
+      <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
+      <c r="O23" s="15"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="16"/>
+      <c r="V23" s="15"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
@@ -1230,28 +1231,28 @@
       <c r="B24" s="2">
         <v>7.3</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="16"/>
+      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="O24" s="15"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="16"/>
+      <c r="V24" s="15"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
@@ -1278,7 +1279,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="16"/>
+      <c r="L25" s="2"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -1288,7 +1289,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="17"/>
+      <c r="V25" s="16"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
@@ -1313,17 +1314,17 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="16"/>
+      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
+      <c r="O26" s="15"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="16"/>
+      <c r="V26" s="15"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
@@ -1348,17 +1349,17 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="16"/>
+      <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
+      <c r="O27" s="15"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="16"/>
+      <c r="V27" s="15"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
@@ -1367,12 +1368,16 @@
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
     </row>
+    <row r="28" spans="1:29">
+      <c r="L28" s="2"/>
+      <c r="O28" s="15"/>
+    </row>
     <row r="29" spans="1:29">
       <c r="A29" s="2">
         <v>9</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="2"/>
@@ -1383,17 +1388,17 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="16"/>
+      <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
+      <c r="O29" s="15"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="16"/>
+      <c r="V29" s="15"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
@@ -1407,7 +1412,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="2"/>
@@ -1418,17 +1423,17 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="16"/>
+      <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
+      <c r="O30" s="15"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="16"/>
+      <c r="V30" s="15"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
@@ -1442,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2"/>
@@ -1453,17 +1458,17 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="16"/>
+      <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
+      <c r="O31" s="15"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-      <c r="V31" s="16"/>
+      <c r="V31" s="15"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
@@ -1477,7 +1482,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1490,17 +1495,17 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="16"/>
+      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="O32" s="15"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="V32" s="16"/>
+      <c r="V32" s="15"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
@@ -1530,7 +1535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add facebook connection API
</commit_message>
<xml_diff>
--- a/_document/Checklist - term2.xlsx
+++ b/_document/Checklist - term2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="120" windowWidth="15255" windowHeight="6045" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="120" windowWidth="15252" windowHeight="6048" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -119,7 +119,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,14 +127,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -546,7 +546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -556,21 +556,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="28.375" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="4.375" customWidth="1"/>
-    <col min="6" max="29" width="3.75" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" customWidth="1"/>
+    <col min="6" max="29" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:31" ht="15">
+    <row r="7" spans="1:31">
       <c r="A7" s="17" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="D17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1535,7 +1535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Checklist term 2
</commit_message>
<xml_diff>
--- a/_document/Checklist - term2.xlsx
+++ b/_document/Checklist - term2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t xml:space="preserve">Facebook Connect </t>
   </si>
@@ -27,9 +27,6 @@
     <t xml:space="preserve">Poll, Quiz </t>
   </si>
   <si>
-    <t>CV, Hobby, relationship…</t>
-  </si>
-  <si>
     <t>Fix lỗi</t>
   </si>
   <si>
@@ -63,15 +60,6 @@
     <t>Some problem with chat module</t>
   </si>
   <si>
-    <t>Tiếp thị hinh ảnh của tổ chức ra bên ngoài</t>
-  </si>
-  <si>
-    <t>Hộp thư nóng, hộp thư ý tưởng…</t>
-  </si>
-  <si>
-    <t>Tuyên dương, phê bình cá nhân tập thể</t>
-  </si>
-  <si>
     <t>Newest friends</t>
   </si>
   <si>
@@ -109,6 +97,27 @@
   </si>
   <si>
     <t>Redirect to nowhere after comment</t>
+  </si>
+  <si>
+    <t>CV, Org profile</t>
+  </si>
+  <si>
+    <t>Thông tin giới thiệu tổ chức</t>
+  </si>
+  <si>
+    <t>Tuyên dương = bài viết</t>
+  </si>
+  <si>
+    <t>Tuyên dương = testimonate: filter by friends, group</t>
+  </si>
+  <si>
+    <t>Tuyên dương bằng rate blog (category Ý tưởng)</t>
+  </si>
+  <si>
+    <t>Ý tưởng và đánh giá</t>
+  </si>
+  <si>
+    <t>Lasted blog by Category</t>
   </si>
 </sst>
 </file>
@@ -223,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -245,8 +254,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,35 +571,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:AE32"/>
+  <dimension ref="A7:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" customWidth="1"/>
     <col min="6" max="29" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:31">
-      <c r="A7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="17"/>
+      <c r="A7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7">
         <v>28</v>
@@ -665,7 +682,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -678,11 +695,11 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="15"/>
+      <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="S8" s="15"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="15"/>
@@ -700,10 +717,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="2"/>
@@ -715,11 +732,11 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="15"/>
+      <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="S9" s="15"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="15"/>
@@ -737,10 +754,10 @@
         <v>1.2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="2"/>
@@ -752,11 +769,11 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="15"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="S10" s="15"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="15"/>
@@ -774,10 +791,10 @@
         <v>1.3</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="2"/>
@@ -789,11 +806,11 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="15"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="15"/>
@@ -811,10 +828,10 @@
         <v>1.4</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -826,11 +843,11 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+      <c r="S12" s="15"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="15"/>
@@ -848,10 +865,10 @@
         <v>1.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="2"/>
@@ -863,11 +880,11 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="15"/>
+      <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="S13" s="15"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="15"/>
@@ -885,10 +902,10 @@
         <v>1.6</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -900,11 +917,11 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="15"/>
+      <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="S14" s="15"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="15"/>
@@ -922,10 +939,10 @@
         <v>1.7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -937,11 +954,11 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="15"/>
+      <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
+      <c r="S15" s="15"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="15"/>
@@ -959,10 +976,10 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
@@ -974,11 +991,11 @@
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="15"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
+      <c r="S16" s="15"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="15"/>
@@ -999,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="3"/>
@@ -1011,11 +1028,11 @@
       <c r="L17" s="3"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="15"/>
+      <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
+      <c r="S17" s="15"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="15"/>
@@ -1036,9 +1053,9 @@
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1048,11 +1065,11 @@
       <c r="L18" s="13"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="15"/>
+      <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
+      <c r="S18" s="15"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="15"/>
@@ -1073,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1089,7 +1106,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
+      <c r="S19" s="15"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="15"/>
@@ -1107,16 +1124,16 @@
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
-      <c r="S20" s="2"/>
+      <c r="S20" s="15"/>
       <c r="V20" s="15"/>
     </row>
     <row r="21" spans="1:29">
@@ -1125,10 +1142,10 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="2"/>
@@ -1162,7 +1179,7 @@
         <v>7.1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1175,13 +1192,13 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
       <c r="V22" s="15"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
@@ -1197,7 +1214,7 @@
         <v>7.2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1210,11 +1227,11 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="15"/>
+      <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
+      <c r="S23" s="15"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="15"/>
@@ -1232,7 +1249,7 @@
         <v>7.3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="15"/>
@@ -1245,11 +1262,11 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="15"/>
+      <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
+      <c r="S24" s="15"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="15"/>
@@ -1267,10 +1284,10 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1304,7 +1321,7 @@
         <v>8.1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1317,11 +1334,11 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="15"/>
+      <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
+      <c r="S26" s="15"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="15"/>
@@ -1339,7 +1356,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1352,11 +1369,11 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="15"/>
+      <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
+      <c r="S27" s="15"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="15"/>
@@ -1370,7 +1387,8 @@
     </row>
     <row r="28" spans="1:29">
       <c r="L28" s="2"/>
-      <c r="O28" s="15"/>
+      <c r="O28" s="2"/>
+      <c r="S28" s="15"/>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="2">
@@ -1378,7 +1396,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1391,11 +1409,11 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="15"/>
+      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
+      <c r="S29" s="15"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="15"/>
@@ -1413,7 +1431,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1426,11 +1444,11 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="15"/>
+      <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="S30" s="15"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="15"/>
@@ -1448,7 +1466,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="10" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1461,11 +1479,11 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="15"/>
+      <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
+      <c r="S31" s="15"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="15"/>
@@ -1479,14 +1497,14 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="9" t="s">
-        <v>3</v>
+      <c r="C32" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1498,11 +1516,11 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="15"/>
+      <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
+      <c r="S32" s="15"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="15"/>
@@ -1513,6 +1531,57 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="20">
+        <v>13</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+    </row>
+    <row r="34" spans="1:29">
+      <c r="A34" s="19">
+        <v>14</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" s="19">
+        <v>15</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
+ Completed CV module + Fix some bugs relate to profile display on wall tab
</commit_message>
<xml_diff>
--- a/_document/Checklist - term2.xlsx
+++ b/_document/Checklist - term2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t xml:space="preserve">Facebook Connect </t>
   </si>
@@ -117,7 +117,19 @@
     <t>Ý tưởng và đánh giá</t>
   </si>
   <si>
-    <t>Lasted blog by Category</t>
+    <t>Organization Photo Gallery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống CMS category </t>
+  </si>
+  <si>
+    <t>Lasted blog entries by Category</t>
+  </si>
+  <si>
+    <t>Register wallpost api</t>
+  </si>
+  <si>
+    <t>Complete wallpost system</t>
   </si>
 </sst>
 </file>
@@ -148,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -257,14 +275,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:AE35"/>
+  <dimension ref="A7:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -588,10 +607,10 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:31">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
@@ -655,7 +674,7 @@
       <c r="W7" s="2">
         <v>14</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="22">
         <v>15</v>
       </c>
       <c r="Y7" s="2">
@@ -699,7 +718,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="15"/>
+      <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="15"/>
@@ -736,7 +755,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="15"/>
+      <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="15"/>
@@ -773,7 +792,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="15"/>
+      <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="15"/>
@@ -810,7 +829,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="15"/>
+      <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="15"/>
@@ -847,7 +866,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="15"/>
+      <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="15"/>
@@ -884,7 +903,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="15"/>
+      <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="15"/>
@@ -921,7 +940,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="15"/>
+      <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="15"/>
@@ -958,7 +977,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="15"/>
+      <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="15"/>
@@ -995,7 +1014,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="15"/>
+      <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="15"/>
@@ -1032,7 +1051,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="15"/>
+      <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="15"/>
@@ -1069,7 +1088,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="15"/>
+      <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="15"/>
@@ -1106,7 +1125,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="15"/>
+      <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="15"/>
@@ -1133,7 +1152,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
-      <c r="S20" s="15"/>
+      <c r="S20" s="2"/>
       <c r="V20" s="15"/>
     </row>
     <row r="21" spans="1:29">
@@ -1196,7 +1215,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="15"/>
+      <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="15"/>
@@ -1231,7 +1250,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="15"/>
+      <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="15"/>
@@ -1266,7 +1285,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="15"/>
+      <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="15"/>
@@ -1338,7 +1357,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="15"/>
+      <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="15"/>
@@ -1373,7 +1392,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="15"/>
+      <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="15"/>
@@ -1388,15 +1407,15 @@
     <row r="28" spans="1:29">
       <c r="L28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="S28" s="15"/>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="2">
         <v>9</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="10" t="s">
-        <v>27</v>
+      <c r="C29" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1413,7 +1432,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="15"/>
+      <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="15"/>
@@ -1430,8 +1449,8 @@
         <v>10</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="10" t="s">
-        <v>29</v>
+      <c r="C30" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1448,7 +1467,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="15"/>
+      <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="15"/>
@@ -1466,7 +1485,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1483,7 +1502,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="15"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="15"/>
@@ -1501,7 +1520,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>22</v>
@@ -1520,7 +1539,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="15"/>
+      <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="15"/>
@@ -1533,12 +1552,12 @@
       <c r="AC32" s="2"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="20">
+      <c r="A33" s="19">
         <v>13</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="21" t="s">
-        <v>32</v>
+      <c r="C33" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1568,19 +1587,51 @@
       <c r="AC33" s="2"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="19">
+      <c r="A34" s="18">
         <v>14</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>33</v>
+      <c r="C34" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:29">
-      <c r="A35" s="19">
+      <c r="A35" s="18">
         <v>15</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" s="18">
+        <v>16</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
+      <c r="A37" s="18">
+        <v>17</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
+      <c r="A38" s="18">
+        <v>18</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29">
+      <c r="A39" s="18">
+        <v>19</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>